<commit_message>
Updated BOM and outline for RGB PCBA
</commit_message>
<xml_diff>
--- a/CAM_OUTPUTS/BOM/RGB_Plugin_Board_CAM_OUTPUT_A2.xlsx
+++ b/CAM_OUTPUTS/BOM/RGB_Plugin_Board_CAM_OUTPUT_A2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\rgb_plugin_pcba\Project Outputs for RGB_Plugin_Board\RGB_Plugin_Board_UPLOAD_GERBERS_A2\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\rgb_plugin_pcba\rgb_plugin_pcba\Project Outputs for RGB_Plugin_Board\RGB_Plugin_Board_UPLOAD_GERBERS_A2\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28635" windowHeight="17115"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22110" windowHeight="14805"/>
   </bookViews>
   <sheets>
     <sheet name="RGB_Plugin_Board_CAM_OUTPUT_A2" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>Comment</t>
   </si>
@@ -68,13 +68,22 @@
     <t>P3</t>
   </si>
   <si>
-    <t>691321100002</t>
-  </si>
-  <si>
-    <t>Serie 3211 - 3.50mm Vertical PCB Header WR-TBL, 2 pin</t>
+    <t>C880557</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Header,Male Pin,Covered(4 Sided) 2 1 0.138"（3.50mm） 2 P=3.5mm Pluggable System Terminal Block RoHS</t>
   </si>
   <si>
     <t>P5</t>
+  </si>
+  <si>
+    <t>SL_3_50_180G_02</t>
+  </si>
+  <si>
+    <t>C192777</t>
   </si>
   <si>
     <t>AO3400A N</t>
@@ -535,44 +544,48 @@
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F3" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="F4" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F5" s="1">
         <v>4</v>
@@ -580,19 +593,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F6" s="1">
         <v>4</v>
@@ -600,19 +613,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="E7" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F7" s="1">
         <v>4</v>
@@ -620,19 +633,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F8" s="1">
         <v>4</v>

</xml_diff>

<commit_message>
Updated BOM for 3.81mm header.
</commit_message>
<xml_diff>
--- a/CAM_OUTPUTS/BOM/RGB_Plugin_Board_CAM_OUTPUT_A2.xlsx
+++ b/CAM_OUTPUTS/BOM/RGB_Plugin_Board_CAM_OUTPUT_A2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\rgb_plugin_pcba\rgb_plugin_pcba\Project Outputs for RGB_Plugin_Board\RGB_Plugin_Board_UPLOAD_GERBERS_A2\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\rgb_plugin_pcba\CAM_OUTPUTS\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -68,9 +68,6 @@
     <t>P3</t>
   </si>
   <si>
-    <t>C880557</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -138,6 +135,9 @@
   </si>
   <si>
     <t>C6649</t>
+  </si>
+  <si>
+    <t>C8391</t>
   </si>
 </sst>
 </file>
@@ -482,7 +482,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -545,7 +547,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
@@ -553,19 +555,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
@@ -573,19 +575,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="F5" s="1">
         <v>4</v>
@@ -593,19 +595,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="F6" s="1">
         <v>4</v>
@@ -613,19 +615,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="F7" s="1">
         <v>4</v>
@@ -633,19 +635,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="F8" s="1">
         <v>4</v>

</xml_diff>